<commit_message>
Actualización - Semana 07
</commit_message>
<xml_diff>
--- a/Presentaciones/ICG/05 - DDA_Bresenham_MidPoint.xlsx
+++ b/Presentaciones/ICG/05 - DDA_Bresenham_MidPoint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositorios\CompuGraph\Repositorio\Presentaciones\ICG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EA53B9-34D8-4281-9726-C36432FFA7F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A904B529-FD35-4078-9FA4-024A10322CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M &gt;= 1" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Bresenham M &lt; 1 (2)" sheetId="7" r:id="rId3"/>
     <sheet name="Bresenham M &lt; 1" sheetId="3" r:id="rId4"/>
     <sheet name="Bresenham M &gt; 1" sheetId="4" r:id="rId5"/>
-    <sheet name="Punto medio Circulo" sheetId="5" r:id="rId6"/>
+    <sheet name="Circulo - Bressenham" sheetId="5" r:id="rId6"/>
     <sheet name="Scan line" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -227,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +324,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -361,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -421,6 +427,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4443,12 +4453,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="O2:V2"/>
-    <mergeCell ref="AA2:AH2"/>
-    <mergeCell ref="AK2:AR2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A8:B8"/>
@@ -4457,6 +4461,12 @@
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="O2:V2"/>
+    <mergeCell ref="AA2:AH2"/>
+    <mergeCell ref="AK2:AR2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4467,8 +4477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AU27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="H1:L10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF18" sqref="AF18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4558,7 +4568,7 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="1">
         <f>C9</f>
         <v>2</v>
       </c>
@@ -4618,14 +4628,14 @@
         <v>-4</v>
       </c>
       <c r="J3" s="4">
-        <f t="shared" ref="J2:J9" si="0">IF(I3&lt;0,I3+$C$7,I3+$C$8)</f>
+        <f t="shared" ref="J3:J9" si="0">IF(I3&lt;0,I3+$C$7,I3+$C$8)</f>
         <v>6</v>
       </c>
       <c r="K3" s="2">
         <f>K2+1</f>
         <v>8</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="42">
         <f>IF(I2&lt;0,L2,L2+1)</f>
         <v>9</v>
       </c>
@@ -4669,8 +4679,8 @@
         <f t="shared" ref="K4:K10" si="2">K3+1</f>
         <v>9</v>
       </c>
-      <c r="L4" s="2">
-        <f t="shared" ref="L4:L10" si="3">IF(I3&lt;0,L3,L3+1)</f>
+      <c r="L4" s="42">
+        <f t="shared" ref="L4:L9" si="3">IF(I3&lt;0,L3,L3+1)</f>
         <v>9</v>
       </c>
       <c r="M4">
@@ -4724,7 +4734,7 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="42">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -4789,7 +4799,7 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="42">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -4857,7 +4867,7 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="42">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -4925,7 +4935,7 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="42">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -4970,11 +4980,11 @@
       <c r="AU8" s="4"/>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9">
+      <c r="B9" s="41"/>
+      <c r="C9" s="1">
         <f>C7-C5</f>
         <v>2</v>
       </c>
@@ -4993,7 +5003,7 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="42">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -5045,7 +5055,7 @@
         <v>15</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="L4:L10" si="4">IF(I9&lt;0,L9,L9+1)</f>
         <v>13</v>
       </c>
       <c r="M10">
@@ -5225,6 +5235,20 @@
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
+      <c r="M14">
+        <v>-8</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
@@ -5240,6 +5264,20 @@
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
+      <c r="M15">
+        <v>-9</v>
+      </c>
+      <c r="N15" s="4"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
@@ -5255,6 +5293,18 @@
     </row>
     <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
+      <c r="M16">
+        <v>-10</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
@@ -5283,6 +5333,18 @@
     </row>
     <row r="17" spans="8:47" x14ac:dyDescent="0.25">
       <c r="H17" s="4"/>
+      <c r="M17">
+        <v>-11</v>
+      </c>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
@@ -5310,6 +5372,18 @@
       <c r="AU17" s="4"/>
     </row>
     <row r="18" spans="8:47" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>-12</v>
+      </c>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="4"/>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
@@ -5337,6 +5411,18 @@
       <c r="AU18" s="4"/>
     </row>
     <row r="19" spans="8:47" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>-13</v>
+      </c>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="1"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
@@ -5364,6 +5450,18 @@
       <c r="AU19" s="4"/>
     </row>
     <row r="20" spans="8:47" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>-14</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
@@ -5391,6 +5489,18 @@
       <c r="AU20" s="4"/>
     </row>
     <row r="21" spans="8:47" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>-15</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
@@ -5418,8 +5528,39 @@
       <c r="AU21" s="4"/>
     </row>
     <row r="22" spans="8:47" x14ac:dyDescent="0.25">
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
+      <c r="N22">
+        <v>7</v>
+      </c>
+      <c r="O22">
+        <v>8</v>
+      </c>
+      <c r="P22">
+        <v>9</v>
+      </c>
+      <c r="Q22">
+        <v>10</v>
+      </c>
+      <c r="R22">
+        <v>11</v>
+      </c>
+      <c r="S22">
+        <v>12</v>
+      </c>
+      <c r="T22">
+        <v>13</v>
+      </c>
+      <c r="U22">
+        <v>14</v>
+      </c>
+      <c r="V22">
+        <v>15</v>
+      </c>
+      <c r="W22">
+        <v>16</v>
+      </c>
+      <c r="X22">
+        <v>17</v>
+      </c>
       <c r="Y22" s="4"/>
       <c r="Z22" s="4"/>
       <c r="AA22" s="4"/>
@@ -6494,8 +6635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AP25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6538,14 +6679,13 @@
       <c r="Q1" s="15"/>
       <c r="R1" s="16"/>
       <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="15"/>
+      <c r="U1" s="27"/>
       <c r="V1" s="27"/>
       <c r="W1" s="17">
         <v>7</v>
       </c>
       <c r="X1" s="17"/>
-      <c r="Y1" s="15"/>
+      <c r="Y1" s="17"/>
       <c r="Z1" s="15"/>
       <c r="AA1" s="15"/>
       <c r="AB1" s="15"/>
@@ -6590,17 +6730,16 @@
       <c r="P2" s="15"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
-      <c r="S2" s="16"/>
+      <c r="S2" s="27"/>
       <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
       <c r="V2" s="15"/>
       <c r="W2" s="15">
         <v>6</v>
       </c>
       <c r="X2" s="15"/>
-      <c r="Y2" s="17"/>
+      <c r="Y2" s="15"/>
       <c r="Z2" s="17"/>
-      <c r="AA2" s="15"/>
+      <c r="AA2" s="17"/>
       <c r="AB2" s="15"/>
       <c r="AC2" s="15"/>
       <c r="AD2" s="15"/>
@@ -6627,14 +6766,13 @@
         <v>1</v>
       </c>
       <c r="L3" s="1">
-        <f>IF(I3&lt;0,L2,L2-1)</f>
+        <f>IF(I2&lt;0,L2,L2-1)</f>
         <v>7</v>
       </c>
       <c r="N3" s="15"/>
       <c r="P3" s="15"/>
       <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="27"/>
+      <c r="R3" s="27"/>
       <c r="T3" s="15"/>
       <c r="U3" s="15"/>
       <c r="V3" s="15"/>
@@ -6644,8 +6782,8 @@
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="15"/>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="17"/>
       <c r="AC3" s="15"/>
       <c r="AD3" s="15"/>
       <c r="AL3" s="15"/>
@@ -6670,20 +6808,20 @@
       </c>
       <c r="J4" s="4">
         <f t="shared" ref="J4:J7" si="2">IF(I4&lt;0,I4+2*K4+2+1,I4+2*K4-2*L4-2)</f>
-        <v>-7.75</v>
+        <v>-9.75</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" ref="K4:K7" si="3">K3+1</f>
         <v>2</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" ref="L4:L7" si="4">IF(I4&lt;0,L3,L3-1)</f>
-        <v>6</v>
+        <f t="shared" ref="L4:L6" si="4">IF(I3&lt;0,L3,L3-1)</f>
+        <v>7</v>
       </c>
       <c r="N4" s="15"/>
       <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="15"/>
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
       <c r="U4" s="15"/>
@@ -6695,8 +6833,7 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="15"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="15"/>
+      <c r="AC4" s="19"/>
       <c r="AD4" s="15"/>
       <c r="AL4" s="15"/>
       <c r="AM4" s="15"/>
@@ -6716,11 +6853,11 @@
       </c>
       <c r="I5" s="5">
         <f t="shared" si="1"/>
-        <v>-7.75</v>
+        <v>-9.75</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" si="2"/>
-        <v>1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="3"/>
@@ -6760,11 +6897,11 @@
       </c>
       <c r="I6" s="5">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="2"/>
-        <v>-2.75</v>
+        <v>10.25</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="3"/>
@@ -6772,11 +6909,11 @@
       </c>
       <c r="L6" s="1">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
@@ -6790,8 +6927,8 @@
       <c r="Z6" s="15"/>
       <c r="AA6" s="15"/>
       <c r="AB6" s="15"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="19"/>
       <c r="AL6" s="15"/>
       <c r="AM6" s="15"/>
       <c r="AN6" s="15"/>
@@ -6807,18 +6944,18 @@
       </c>
       <c r="I7" s="5">
         <f t="shared" si="1"/>
-        <v>-2.75</v>
+        <v>10.25</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="2"/>
-        <v>10.25</v>
+        <v>8.25</v>
       </c>
       <c r="K7" s="18">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L7" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="L4:L7" si="5">IF(I7&lt;0,L6,L6-1)</f>
         <v>5</v>
       </c>
       <c r="N7" s="15"/>
@@ -6856,7 +6993,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="N8" s="15"/>
-      <c r="P8" s="29">
+      <c r="P8" s="20">
         <v>-7</v>
       </c>
       <c r="Q8" s="15">
@@ -6939,8 +7076,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="28"/>
+      <c r="P10" s="28"/>
       <c r="R10" s="15"/>
       <c r="S10" s="16"/>
       <c r="T10" s="16"/>
@@ -6954,8 +7090,7 @@
       <c r="Z10" s="15"/>
       <c r="AA10" s="15"/>
       <c r="AB10" s="15"/>
-      <c r="AC10" s="22"/>
-      <c r="AD10" s="15"/>
+      <c r="AD10" s="22"/>
       <c r="AL10" s="15"/>
       <c r="AM10" s="15"/>
       <c r="AN10" s="16"/>
@@ -6996,8 +7131,8 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="16"/>
       <c r="S12" s="16"/>
       <c r="T12" s="16"/>
       <c r="U12" s="15"/>
@@ -7009,8 +7144,7 @@
       <c r="Y12" s="15"/>
       <c r="Z12" s="15"/>
       <c r="AA12" s="15"/>
-      <c r="AB12" s="22"/>
-      <c r="AC12" s="15"/>
+      <c r="AC12" s="22"/>
       <c r="AD12" s="15"/>
       <c r="AL12" s="15"/>
       <c r="AM12" s="15"/>
@@ -7026,8 +7160,7 @@
       <c r="J13" s="4"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="26"/>
+      <c r="R13" s="26"/>
       <c r="T13" s="16"/>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
@@ -7037,8 +7170,7 @@
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
-      <c r="AA13" s="24"/>
-      <c r="AB13" s="15"/>
+      <c r="AB13" s="24"/>
       <c r="AC13" s="15"/>
       <c r="AD13" s="15"/>
       <c r="AL13" s="15"/>
@@ -7054,17 +7186,15 @@
       <c r="P14" s="15"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
+      <c r="S14" s="26"/>
       <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
       <c r="V14" s="15"/>
       <c r="W14" s="15">
         <v>-6</v>
       </c>
       <c r="X14" s="15"/>
-      <c r="Y14" s="24"/>
       <c r="Z14" s="24"/>
-      <c r="AA14" s="15"/>
+      <c r="AA14" s="24"/>
       <c r="AB14" s="15"/>
       <c r="AC14" s="15"/>
       <c r="AD14" s="15"/>
@@ -7083,11 +7213,13 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
+      <c r="U15" s="26"/>
       <c r="V15" s="25"/>
       <c r="W15" s="24">
         <v>-7</v>
       </c>
       <c r="X15" s="23"/>
+      <c r="Y15" s="24"/>
       <c r="AD15" s="4"/>
       <c r="AL15" s="4"/>
       <c r="AM15" s="4"/>
@@ -7237,11 +7369,11 @@
       </c>
       <c r="Y20" s="4"/>
       <c r="Z20" s="29">
-        <f t="shared" ref="Z20:AA24" si="5">K2*-1</f>
+        <f t="shared" ref="Z20:AA24" si="6">K2*-1</f>
         <v>0</v>
       </c>
       <c r="AA20" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-7</v>
       </c>
       <c r="AC20" s="4">
@@ -7302,11 +7434,11 @@
       </c>
       <c r="Y21" s="4"/>
       <c r="Z21" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="AA21" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-7</v>
       </c>
       <c r="AC21" s="30">
@@ -7335,7 +7467,7 @@
     <row r="22" spans="8:42" x14ac:dyDescent="0.25">
       <c r="N22" s="6">
         <f>L4</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O22" s="6">
         <f>K4</f>
@@ -7343,7 +7475,7 @@
       </c>
       <c r="Q22" s="21">
         <f>L4</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R22" s="21">
         <f>K4*-1</f>
@@ -7355,11 +7487,11 @@
       </c>
       <c r="U22" s="23">
         <f>L4*-1</f>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="W22" s="25">
         <f>L4*-1</f>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="X22" s="25">
         <f>K4*-1</f>
@@ -7367,16 +7499,16 @@
       </c>
       <c r="Y22" s="4"/>
       <c r="Z22" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2</v>
       </c>
       <c r="AA22" s="29">
-        <f t="shared" si="5"/>
-        <v>-6</v>
+        <f t="shared" si="6"/>
+        <v>-7</v>
       </c>
       <c r="AC22" s="30">
         <f>L4*-1</f>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="AD22" s="30">
         <f>K4</f>
@@ -7384,7 +7516,7 @@
       </c>
       <c r="AF22" s="31">
         <f>L4</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AG22" s="31">
         <f>K4*-1</f>
@@ -7432,11 +7564,11 @@
       </c>
       <c r="Y23" s="4"/>
       <c r="Z23" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-3</v>
       </c>
       <c r="AA23" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-6</v>
       </c>
       <c r="AC23" s="30">
@@ -7465,7 +7597,7 @@
     <row r="24" spans="8:42" x14ac:dyDescent="0.25">
       <c r="N24" s="6">
         <f>L6</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O24" s="6">
         <f>K6</f>
@@ -7473,7 +7605,7 @@
       </c>
       <c r="Q24" s="21">
         <f>L6</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R24" s="21">
         <f>K6*-1</f>
@@ -7485,11 +7617,11 @@
       </c>
       <c r="U24">
         <f>L6*-1</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="W24" s="25">
         <f>L6*-1</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="X24" s="25">
         <f>K6*-1</f>
@@ -7497,16 +7629,16 @@
       </c>
       <c r="Y24" s="4"/>
       <c r="Z24" s="29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-4</v>
       </c>
       <c r="AA24" s="29">
-        <f t="shared" si="5"/>
-        <v>-5</v>
+        <f t="shared" si="6"/>
+        <v>-6</v>
       </c>
       <c r="AC24" s="30">
         <f>L6*-1</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="AD24" s="30">
         <f>K6</f>
@@ -7514,7 +7646,7 @@
       </c>
       <c r="AF24" s="31">
         <f>L6</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AG24" s="31">
         <f>K6*-1</f>

</xml_diff>